<commit_message>
chore: commit local changes
</commit_message>
<xml_diff>
--- a/assets/templates/Financial_Model_SAMPLE_DEMO_USD_thousands_GAAP.xlsx
+++ b/assets/templates/Financial_Model_SAMPLE_DEMO_USD_thousands_GAAP.xlsx
@@ -1848,7 +1848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
@@ -1859,6 +1859,7 @@
   <cols>
     <col width="41.1796875" customWidth="1" style="14" min="1" max="1"/>
     <col width="13.08984375" customWidth="1" style="14" min="2" max="9"/>
+    <col hidden="1" width="13" customWidth="1" min="5" max="5"/>
     <col width="2.36328125" customWidth="1" style="14" min="10" max="10"/>
     <col width="34.54296875" customWidth="1" style="14" min="11" max="11"/>
     <col width="9.08984375" customWidth="1" style="14" min="12" max="16384"/>
@@ -1893,7 +1894,7 @@
     <row r="3" ht="14.5" customFormat="1" customHeight="1" s="58">
       <c r="A3" s="59" t="inlineStr">
         <is>
-          <t>Balance Sheet Check (A - L + E)</t>
+          <t>Balance Sheet Check (A - (L + E))</t>
         </is>
       </c>
       <c r="B3" s="92">
@@ -2974,15 +2975,13 @@
         </is>
       </c>
       <c r="B77" s="105" t="n">
-        <v>73.10000000000002</v>
-      </c>
-      <c r="C77" s="97">
-        <f>B77+C43-C45</f>
-        <v/>
-      </c>
-      <c r="D77" s="97">
-        <f>C77+D43-D45</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="C77" s="105" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="105" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78" outlineLevel="1" ht="14.5" customHeight="1">

</xml_diff>